<commit_message>
Add nrel submission file.
</commit_message>
<xml_diff>
--- a/quantum_hardware_testing_20250501.xlsx
+++ b/quantum_hardware_testing_20250501.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chl23026\Nutstore\1\Nutstore\Workspace\quantum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9D9CD7-4738-472F-ABEC-09A748790A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC115A85-408E-42FD-A092-B2B9D7B97FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="IBM hardware 20250501" sheetId="1" r:id="rId1"/>
+    <sheet name="AER" sheetId="2" r:id="rId2"/>
+    <sheet name="Simulator" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -211,15 +213,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,14 +788,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>16772519</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="H13" s="5"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -843,4 +844,28 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8FD886-4C40-49BC-80B6-A8808BDAD017}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F71AD9-B153-47BF-A3B6-15219E952424}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix the timing and typo in PauliTwoDesign ansatz
</commit_message>
<xml_diff>
--- a/quantum_hardware_testing_20250501.xlsx
+++ b/quantum_hardware_testing_20250501.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chl23026\Nutstore\1\Nutstore\Workspace\quantum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0642F7-9C0E-4B2A-A8EF-E0E8D38D476C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E9A152-D2A8-4A12-A010-7E7B16C8F6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="72">
   <si>
     <t>This is the testing of main_VQE_heat.py code on the IBM quantum hardware for backend1 option</t>
   </si>
@@ -226,6 +226,24 @@
   </si>
   <si>
     <t>memory usage</t>
+  </si>
+  <si>
+    <t>928KB</t>
+  </si>
+  <si>
+    <t>936KB</t>
+  </si>
+  <si>
+    <t>8.56GB</t>
+  </si>
+  <si>
+    <t>241.67MB</t>
+  </si>
+  <si>
+    <t>1.16MB</t>
+  </si>
+  <si>
+    <t>8.87GB</t>
   </si>
 </sst>
 </file>
@@ -911,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE26B11F-50C5-4099-8A83-9E9E20D94F52}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +942,7 @@
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" customWidth="1"/>
     <col min="11" max="11" width="20.140625" customWidth="1"/>
@@ -984,6 +1002,27 @@
       <c r="E2" t="s">
         <v>52</v>
       </c>
+      <c r="F2">
+        <v>250.5</v>
+      </c>
+      <c r="G2">
+        <v>1.28</v>
+      </c>
+      <c r="H2">
+        <v>9.8620000000000001</v>
+      </c>
+      <c r="I2">
+        <v>8.2600000000000002E-4</v>
+      </c>
+      <c r="J2">
+        <v>9.8620000000000001</v>
+      </c>
+      <c r="K2">
+        <v>3.3500000000000001E-3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1001,6 +1040,15 @@
       <c r="E3" t="s">
         <v>53</v>
       </c>
+      <c r="F3">
+        <v>127.9</v>
+      </c>
+      <c r="G3">
+        <v>4.78</v>
+      </c>
+      <c r="L3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1018,6 +1066,15 @@
       <c r="E4" t="s">
         <v>54</v>
       </c>
+      <c r="F4">
+        <v>16.149999999999999</v>
+      </c>
+      <c r="G4">
+        <v>21.12</v>
+      </c>
+      <c r="L4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1035,6 +1092,15 @@
       <c r="E5" t="s">
         <v>55</v>
       </c>
+      <c r="F5">
+        <v>33.369999999999997</v>
+      </c>
+      <c r="G5">
+        <v>282.83999999999997</v>
+      </c>
+      <c r="L5" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1052,10 +1118,19 @@
       <c r="E6" t="s">
         <v>51</v>
       </c>
+      <c r="F6">
+        <v>18.829999999999998</v>
+      </c>
+      <c r="G6">
+        <v>1778.83</v>
+      </c>
+      <c r="L6" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>18994236</v>
+        <v>18994401</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -1069,10 +1144,19 @@
       <c r="E7" t="s">
         <v>52</v>
       </c>
+      <c r="F7">
+        <v>746.3</v>
+      </c>
+      <c r="G7">
+        <v>1.44</v>
+      </c>
+      <c r="L7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>18994250</v>
+        <v>18994593</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -1086,10 +1170,19 @@
       <c r="E8" t="s">
         <v>53</v>
       </c>
+      <c r="F8">
+        <v>106.1</v>
+      </c>
+      <c r="G8">
+        <v>5.61</v>
+      </c>
+      <c r="L8" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>18994251</v>
+        <v>18994600</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -1103,8 +1196,20 @@
       <c r="E9" t="s">
         <v>54</v>
       </c>
+      <c r="F9">
+        <v>10.09</v>
+      </c>
+      <c r="G9">
+        <v>23.83</v>
+      </c>
+      <c r="L9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>18994607</v>
+      </c>
       <c r="B10">
         <v>5</v>
       </c>
@@ -1117,8 +1222,20 @@
       <c r="E10" t="s">
         <v>55</v>
       </c>
+      <c r="F10">
+        <v>31.29</v>
+      </c>
+      <c r="G10">
+        <v>382.37</v>
+      </c>
+      <c r="L10" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>18994609</v>
+      </c>
       <c r="B11">
         <v>5</v>
       </c>

</xml_diff>